<commit_message>
updateds beihai dates to match 2021
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07660D7D-4592-4C7C-8F8F-A5BE27D5B52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A81ED8-4226-4A09-809F-A8BDCF8D3BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>aguasclaras_buffed</t>
+  </si>
+  <si>
+    <t>('2017-03-07','2017-04-07')</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1431,7 +1434,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>25</v>
@@ -1484,7 +1487,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
changed cloud cover to 0.5
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A81ED8-4226-4A09-809F-A8BDCF8D3BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DEDF82-8438-4E55-A8A9-5E4CE712A327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROIs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>('2017-03-07','2017-04-07')</t>
+  </si>
+  <si>
+    <t>('2017-03-07','2017-05-07')</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1178,7 +1181,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
@@ -1231,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="4">
         <v>5</v>
@@ -1284,7 +1287,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="4">
         <v>5</v>
@@ -1337,7 +1340,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="4">
         <v>5</v>
@@ -1390,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="4">
         <v>5</v>
@@ -1443,7 +1446,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="4">
         <v>5</v>
@@ -1496,7 +1499,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
@@ -1549,7 +1552,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
@@ -1602,7 +1605,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="4">
         <v>5</v>
@@ -1655,7 +1658,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="4">
         <v>5</v>
@@ -1708,7 +1711,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="4">
         <v>5</v>
@@ -1763,7 +1766,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H13" s="4">
         <v>5</v>
@@ -1818,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="4">
         <v>5</v>
@@ -1873,7 +1876,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -1928,7 +1931,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="4">
         <v>5</v>
@@ -1981,7 +1984,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H17" s="4">
         <v>5</v>
@@ -2025,7 +2028,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>25</v>
@@ -2034,7 +2037,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H18" s="4">
         <v>5</v>
@@ -2078,7 +2081,7 @@
         <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>25</v>
@@ -2087,7 +2090,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H19" s="4">
         <v>5</v>
@@ -2140,7 +2143,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H20" s="4">
         <v>5</v>
@@ -2193,7 +2196,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="4">
         <v>5</v>
@@ -2246,7 +2249,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H22" s="4">
         <v>5</v>
@@ -2299,7 +2302,7 @@
         <v>15</v>
       </c>
       <c r="G23" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H23" s="4">
         <v>5</v>
@@ -2352,7 +2355,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H24" s="4">
         <v>5</v>
@@ -2405,7 +2408,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H25" s="4">
         <v>5</v>
@@ -2458,7 +2461,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H26" s="4">
         <v>5</v>
@@ -2513,7 +2516,7 @@
         <v>15</v>
       </c>
       <c r="G27" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="4">
         <v>5</v>
@@ -2566,7 +2569,7 @@
         <v>15</v>
       </c>
       <c r="G28" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H28" s="4">
         <v>5</v>
@@ -2619,7 +2622,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H29" s="4">
         <v>5</v>
@@ -2674,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="G30" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H30" s="4">
         <v>5</v>
@@ -2727,7 +2730,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H31" s="4">
         <v>5</v>
@@ -2780,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="G32" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="4">
         <v>5</v>
@@ -2833,7 +2836,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H33" s="4">
         <v>5</v>
@@ -2886,7 +2889,7 @@
         <v>15</v>
       </c>
       <c r="G34" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H34" s="4">
         <v>5</v>
@@ -2939,7 +2942,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
@@ -2992,7 +2995,7 @@
         <v>15</v>
       </c>
       <c r="G36" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H36" s="4">
         <v>5</v>
@@ -3045,7 +3048,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
@@ -3098,7 +3101,7 @@
         <v>15</v>
       </c>
       <c r="G38" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
@@ -3151,7 +3154,7 @@
         <v>15</v>
       </c>
       <c r="G39" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H39" s="4">
         <v>5</v>
@@ -3204,7 +3207,7 @@
         <v>15</v>
       </c>
       <c r="G40" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H40" s="4">
         <v>5</v>
@@ -3257,7 +3260,7 @@
         <v>15</v>
       </c>
       <c r="G41" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H41" s="4">
         <v>5</v>
@@ -3310,7 +3313,7 @@
         <v>15</v>
       </c>
       <c r="G42" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H42" s="4">
         <v>5</v>
@@ -3363,7 +3366,7 @@
         <v>15</v>
       </c>
       <c r="G43" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H43" s="4">
         <v>5</v>
@@ -3418,7 +3421,7 @@
         <v>15</v>
       </c>
       <c r="G44" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H44" s="4">
         <v>5</v>
@@ -3471,7 +3474,7 @@
         <v>15</v>
       </c>
       <c r="G45" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H45" s="4">
         <v>5</v>
@@ -3524,7 +3527,7 @@
         <v>15</v>
       </c>
       <c r="G46" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H46" s="4">
         <v>5</v>
@@ -3577,7 +3580,7 @@
         <v>15</v>
       </c>
       <c r="G47" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H47" s="4">
         <v>5</v>

</xml_diff>

<commit_message>
updated rois and dates
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF687D1-94D0-4859-94DF-D50AC60AF069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07957113-F0A7-4880-8777-A41C60C040F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -363,9 +363,6 @@
     <t>('2017-07-07','2017-08-07')</t>
   </si>
   <si>
-    <t>('2017-01-07','2017-02-07')</t>
-  </si>
-  <si>
     <t>special case, coverege in rio is weird in 2022 so we chose 2017 instead</t>
   </si>
   <si>
@@ -381,19 +378,34 @@
     <t>aguasclaras</t>
   </si>
   <si>
-    <t>('2021-06-07','2021-07-07')</t>
-  </si>
-  <si>
     <t>aguasclaras_buffed</t>
-  </si>
-  <si>
-    <t>('2017-03-07','2017-04-07')</t>
   </si>
   <si>
     <t>('2017-03-07','2017-05-07')</t>
   </si>
   <si>
-    <t>('2017-04-07','2017-06-07')</t>
+    <t>[[[54.540252685546875,24.291407914292037],[54.61406707763672,24.291407914292037],[54.61406707763672,24.366488081551143],[54.540252685546875,24.366488081551143],[54.540252685546875,24.291407914292037]]]</t>
+  </si>
+  <si>
+    <t>[[[54.453049, 24.297666], [54.453049, 24.444649], [54.700241, 24.444649], [54.700241, 24.297666], [54.453049, 24.297666]]]</t>
+  </si>
+  <si>
+    <t>[[[55.201492, 25.149014], [55.201492, 25.287542], [55.440445, 25.287542], [55.440445, 25.149014], [55.201492, 25.149014]]]</t>
+  </si>
+  <si>
+    <t>('2017-01-07','2017-03-17')</t>
+  </si>
+  <si>
+    <t>('2017-04-07','2017-07-07')</t>
+  </si>
+  <si>
+    <t>('2017-06-07','2017-09-07')</t>
+  </si>
+  <si>
+    <t>('2017-03-07','2017-06-07')</t>
+  </si>
+  <si>
+    <t>('2017-05-07','2017-07-07')</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1144,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>11</v>
@@ -1172,7 +1184,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>109</v>
@@ -1199,7 +1211,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1225,7 +1237,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>109</v>
@@ -1252,7 +1264,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1272,7 +1284,7 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="4">
         <v>17</v>
@@ -1281,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>14</v>
@@ -1305,7 +1317,7 @@
         <v>16</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1325,7 +1337,7 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B5" s="4">
         <v>17</v>
@@ -1334,7 +1346,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>14</v>
@@ -1358,7 +1370,7 @@
         <v>19</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1411,7 +1423,7 @@
         <v>22</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1440,7 +1452,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>25</v>
@@ -1449,7 +1461,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="4">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H7" s="4">
         <v>5</v>
@@ -1464,7 +1476,7 @@
         <v>16</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1493,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>25</v>
@@ -1502,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
@@ -1517,7 +1529,7 @@
         <v>19</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1546,7 +1558,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
@@ -1555,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
@@ -1570,7 +1582,7 @@
         <v>22</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1599,7 +1611,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>25</v>
@@ -1608,7 +1620,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <v>5</v>
@@ -1623,7 +1635,7 @@
         <v>16</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1676,7 +1688,7 @@
         <v>22</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -1705,7 +1717,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1714,7 +1726,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
         <v>5</v>
@@ -1729,7 +1741,7 @@
         <v>16</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>36</v>
@@ -1760,7 +1772,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>14</v>
@@ -1769,7 +1781,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4">
         <v>5</v>
@@ -1784,7 +1796,7 @@
         <v>19</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>36</v>
@@ -1839,7 +1851,7 @@
         <v>16</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>41</v>
@@ -1894,7 +1906,7 @@
         <v>19</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>41</v>
@@ -1949,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -2002,7 +2014,7 @@
         <v>19</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -2031,7 +2043,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>25</v>
@@ -2055,7 +2067,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -2084,7 +2096,7 @@
         <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>25</v>
@@ -2108,7 +2120,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2161,7 +2173,7 @@
         <v>16</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2214,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2267,7 +2279,7 @@
         <v>22</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -2320,7 +2332,7 @@
         <v>16</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2373,7 +2385,7 @@
         <v>19</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -2399,7 +2411,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>109</v>
@@ -2426,7 +2438,7 @@
         <v>22</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -2479,7 +2491,7 @@
         <v>16</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>65</v>
@@ -2534,7 +2546,7 @@
         <v>22</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -2587,7 +2599,7 @@
         <v>16</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -2640,7 +2652,7 @@
         <v>19</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>72</v>
@@ -2695,7 +2707,7 @@
         <v>16</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2748,7 +2760,7 @@
         <v>19</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2801,7 +2813,7 @@
         <v>16</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2854,7 +2866,7 @@
         <v>19</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2883,7 +2895,7 @@
         <v>82</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>14</v>
@@ -2892,7 +2904,7 @@
         <v>15</v>
       </c>
       <c r="G34" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H34" s="4">
         <v>5</v>
@@ -2907,7 +2919,7 @@
         <v>16</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2936,7 +2948,7 @@
         <v>84</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>14</v>
@@ -2945,7 +2957,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
@@ -2960,7 +2972,7 @@
         <v>19</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -3013,7 +3025,7 @@
         <v>16</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -3066,7 +3078,7 @@
         <v>19</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -3095,7 +3107,7 @@
         <v>90</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>14</v>
@@ -3104,7 +3116,7 @@
         <v>15</v>
       </c>
       <c r="G38" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
@@ -3119,7 +3131,7 @@
         <v>16</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3172,7 +3184,7 @@
         <v>16</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -3225,7 +3237,7 @@
         <v>19</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -3278,7 +3290,7 @@
         <v>16</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -3331,7 +3343,7 @@
         <v>16</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -3384,10 +3396,10 @@
         <v>16</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -3439,7 +3451,7 @@
         <v>16</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -3492,7 +3504,7 @@
         <v>16</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
@@ -3545,7 +3557,7 @@
         <v>16</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -3598,7 +3610,7 @@
         <v>19</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
@@ -31366,17 +31378,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:H40 F42:H43">
+  <conditionalFormatting sqref="F42:H43 F34:H40">
     <cfRule type="expression" dxfId="41" priority="9">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:H40 F42:H43">
+  <conditionalFormatting sqref="F42:H43 F34:H40">
     <cfRule type="expression" dxfId="40" priority="10">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:H40 F42:H43">
+  <conditionalFormatting sqref="F42:H43 F34:H40">
     <cfRule type="expression" dxfId="39" priority="11">
       <formula>#REF!="main"</formula>
     </cfRule>

</xml_diff>

<commit_message>
added dupllicated cell value red highlit to roi column
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07957113-F0A7-4880-8777-A41C60C040F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D029447-4BFB-42AC-A874-B1C75DE71B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,7 +502,401 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="97">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAADB"/>
+          <bgColor rgb="FF8EAADB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2CB"/>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1100,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -31325,22 +31719,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="47" priority="1">
+    <cfRule type="expression" dxfId="96" priority="2">
       <formula>$K2="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="95" priority="3">
       <formula>$K2="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="45" priority="3">
+    <cfRule type="expression" dxfId="94" priority="4">
       <formula>$K2="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1002">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31352,22 +31746,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="44" priority="5">
+    <cfRule type="expression" dxfId="93" priority="6">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="43" priority="6">
+    <cfRule type="expression" dxfId="92" priority="7">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="42" priority="7">
+    <cfRule type="expression" dxfId="91" priority="8">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1002">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31379,214 +31773,217 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="41" priority="9">
+    <cfRule type="expression" dxfId="90" priority="10">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="40" priority="10">
+    <cfRule type="expression" dxfId="89" priority="11">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="39" priority="11">
+    <cfRule type="expression" dxfId="88" priority="12">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="38" priority="12">
+    <cfRule type="expression" dxfId="87" priority="13">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="86" priority="14">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="36" priority="14">
+    <cfRule type="expression" dxfId="85" priority="15">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="35" priority="15">
+    <cfRule type="expression" dxfId="84" priority="16">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="34" priority="16">
+    <cfRule type="expression" dxfId="83" priority="17">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="82" priority="18">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="32" priority="18">
+    <cfRule type="expression" dxfId="81" priority="19">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="31" priority="19">
+    <cfRule type="expression" dxfId="80" priority="20">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="79" priority="21">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="29" priority="21">
+    <cfRule type="expression" dxfId="78" priority="22">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="28" priority="22">
+    <cfRule type="expression" dxfId="77" priority="23">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="27" priority="23">
+    <cfRule type="expression" dxfId="76" priority="24">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="26" priority="24">
+    <cfRule type="expression" dxfId="75" priority="25">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="25" priority="25">
+    <cfRule type="expression" dxfId="74" priority="26">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="73" priority="27">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="72" priority="28">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="71" priority="29">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="21" priority="29">
+    <cfRule type="expression" dxfId="70" priority="30">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="20" priority="30">
+    <cfRule type="expression" dxfId="69" priority="31">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="19" priority="31">
+    <cfRule type="expression" dxfId="68" priority="32">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="18" priority="32">
+    <cfRule type="expression" dxfId="67" priority="33">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="17" priority="33">
+    <cfRule type="expression" dxfId="66" priority="34">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="16" priority="34">
+    <cfRule type="expression" dxfId="65" priority="35">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="15" priority="35">
+    <cfRule type="expression" dxfId="64" priority="36">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="14" priority="36">
+    <cfRule type="expression" dxfId="63" priority="37">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="13" priority="37">
+    <cfRule type="expression" dxfId="62" priority="38">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="12" priority="38">
+    <cfRule type="expression" dxfId="61" priority="39">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="11" priority="39">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="10" priority="40">
+    <cfRule type="expression" dxfId="59" priority="41">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="9" priority="41">
+    <cfRule type="expression" dxfId="58" priority="42">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="8" priority="42">
+    <cfRule type="expression" dxfId="57" priority="43">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="7" priority="43">
+    <cfRule type="expression" dxfId="56" priority="44">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="6" priority="44">
+    <cfRule type="expression" dxfId="55" priority="45">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="5" priority="45">
+    <cfRule type="expression" dxfId="54" priority="46">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="4" priority="46">
+    <cfRule type="expression" dxfId="53" priority="47">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="3" priority="47">
+    <cfRule type="expression" dxfId="52" priority="48">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="2" priority="48">
+    <cfRule type="expression" dxfId="51" priority="49">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="50" priority="50">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="0" priority="50">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>#REF!="main"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated beihi adj date and cloud
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D029447-4BFB-42AC-A874-B1C75DE71B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE931F-5F6D-4B97-B185-DF401410CC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,10 +402,10 @@
     <t>('2017-06-07','2017-09-07')</t>
   </si>
   <si>
-    <t>('2017-03-07','2017-06-07')</t>
+    <t>('2017-05-07','2017-07-07')</t>
   </si>
   <si>
-    <t>('2017-05-07','2017-07-07')</t>
+    <t>('2017-08-01','2017-11-07')</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
+  <dxfs count="49">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -510,390 +510,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAADB"/>
-          <bgColor rgb="FF8EAADB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1495,7 +1111,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1846,7 +1462,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>25</v>
@@ -1855,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H7" s="4">
         <v>5</v>
@@ -1908,7 +1524,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
@@ -1952,7 +1568,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
@@ -1961,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
@@ -3501,7 +3117,7 @@
         <v>90</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>14</v>
@@ -31719,17 +31335,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="96" priority="2">
+    <cfRule type="expression" dxfId="48" priority="2">
       <formula>$K2="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="95" priority="3">
+    <cfRule type="expression" dxfId="47" priority="3">
       <formula>$K2="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L1002">
-    <cfRule type="expression" dxfId="94" priority="4">
+    <cfRule type="expression" dxfId="46" priority="4">
       <formula>$K2="main"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31746,17 +31362,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="93" priority="6">
+    <cfRule type="expression" dxfId="45" priority="6">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="92" priority="7">
+    <cfRule type="expression" dxfId="44" priority="7">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="91" priority="8">
+    <cfRule type="expression" dxfId="43" priority="8">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31773,212 +31389,212 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="90" priority="10">
+    <cfRule type="expression" dxfId="42" priority="10">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="89" priority="11">
+    <cfRule type="expression" dxfId="41" priority="11">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="88" priority="12">
+    <cfRule type="expression" dxfId="40" priority="12">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="87" priority="13">
+    <cfRule type="expression" dxfId="39" priority="13">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="86" priority="14">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="85" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="84" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="83" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="82" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="81" priority="19">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="80" priority="20">
+    <cfRule type="expression" dxfId="32" priority="20">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="79" priority="21">
+    <cfRule type="expression" dxfId="31" priority="21">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="78" priority="22">
+    <cfRule type="expression" dxfId="30" priority="22">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="77" priority="23">
+    <cfRule type="expression" dxfId="29" priority="23">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="76" priority="24">
+    <cfRule type="expression" dxfId="28" priority="24">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="75" priority="25">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="74" priority="26">
+    <cfRule type="expression" dxfId="26" priority="26">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="73" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="72" priority="28">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="71" priority="29">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="70" priority="30">
+    <cfRule type="expression" dxfId="22" priority="30">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="69" priority="31">
+    <cfRule type="expression" dxfId="21" priority="31">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="68" priority="32">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="67" priority="33">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="66" priority="34">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="65" priority="35">
+    <cfRule type="expression" dxfId="17" priority="35">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="64" priority="36">
+    <cfRule type="expression" dxfId="16" priority="36">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="63" priority="37">
+    <cfRule type="expression" dxfId="15" priority="37">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="62" priority="38">
+    <cfRule type="expression" dxfId="14" priority="38">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="61" priority="39">
+    <cfRule type="expression" dxfId="13" priority="39">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="60" priority="40">
+    <cfRule type="expression" dxfId="12" priority="40">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="59" priority="41">
+    <cfRule type="expression" dxfId="11" priority="41">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="58" priority="42">
+    <cfRule type="expression" dxfId="10" priority="42">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="57" priority="43">
+    <cfRule type="expression" dxfId="9" priority="43">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="56" priority="44">
+    <cfRule type="expression" dxfId="8" priority="44">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="55" priority="45">
+    <cfRule type="expression" dxfId="7" priority="45">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="54" priority="46">
+    <cfRule type="expression" dxfId="6" priority="46">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="53" priority="47">
+    <cfRule type="expression" dxfId="5" priority="47">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="52" priority="48">
+    <cfRule type="expression" dxfId="4" priority="48">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="51" priority="49">
+    <cfRule type="expression" dxfId="3" priority="49">
       <formula>#REF!="adj"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="50" priority="50">
+    <cfRule type="expression" dxfId="2" priority="50">
       <formula>#REF!="buff"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="49" priority="51">
+    <cfRule type="expression" dxfId="1" priority="51">
       <formula>#REF!="main"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
removed beihi adj it was too much of a problem
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE931F-5F6D-4B97-B185-DF401410CC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3E8A3-4B2D-438C-BDE5-2B21F3C5D55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="124">
   <si>
     <t>name</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>[[[109.386406, 21.472559], [109.386406, 21.616579], [109.556351, 21.616579], [109.556351, 21.472559], [109.386406, 21.472559]]]</t>
-  </si>
-  <si>
-    <t>beihai_adj_gaoqiazhen</t>
-  </si>
-  <si>
-    <t>[[[109.632225, 21.592639], [109.632225, 21.756311], [109.816246, 21.756311], [109.816246, 21.592639], [109.632225, 21.592639]]]</t>
   </si>
   <si>
     <t>beirut</t>
@@ -403,9 +397,6 @@
   </si>
   <si>
     <t>('2017-05-07','2017-07-07')</t>
-  </si>
-  <si>
-    <t>('2017-08-01','2017-11-07')</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1002"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1157,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>11</v>
@@ -1194,10 +1185,10 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
@@ -1221,7 +1212,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1247,10 +1238,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1274,7 +1265,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1294,7 +1285,7 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="4">
         <v>17</v>
@@ -1303,7 +1294,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>14</v>
@@ -1327,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1347,7 +1338,7 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="4">
         <v>17</v>
@@ -1356,7 +1347,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>14</v>
@@ -1380,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1409,7 +1400,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>14</v>
@@ -1433,7 +1424,7 @@
         <v>22</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1462,7 +1453,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>25</v>
@@ -1486,7 +1477,7 @@
         <v>16</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1515,7 +1506,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>25</v>
@@ -1539,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1568,7 +1559,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
@@ -1577,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
@@ -1589,10 +1580,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1621,7 +1612,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>25</v>
@@ -1630,7 +1621,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="4">
         <v>5</v>
@@ -1642,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1674,16 +1665,16 @@
         <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <v>5</v>
@@ -1695,12 +1686,14 @@
         <v>0</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M11" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -1718,16 +1711,16 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4">
         <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1748,13 +1741,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1782,7 +1775,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>14</v>
@@ -1791,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H13" s="4">
         <v>5</v>
@@ -1803,13 +1796,13 @@
         <v>0</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1828,16 +1821,16 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>14</v>
@@ -1858,13 +1851,13 @@
         <v>0</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1892,7 +1885,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>14</v>
@@ -1910,17 +1903,15 @@
         <v>1</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1947,7 +1938,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>14</v>
@@ -1968,10 +1959,10 @@
         <v>18</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -2000,10 +1991,10 @@
         <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>15</v>
@@ -2021,10 +2012,10 @@
         <v>18</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -2053,7 +2044,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>25</v>
@@ -2074,10 +2065,10 @@
         <v>18</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -2106,10 +2097,10 @@
         <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>15</v>
@@ -2127,10 +2118,10 @@
         <v>18</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2159,7 +2150,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>14</v>
@@ -2180,10 +2171,10 @@
         <v>18</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2212,7 +2203,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>14</v>
@@ -2230,13 +2221,13 @@
         <v>1</v>
       </c>
       <c r="J21" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2265,7 +2256,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>14</v>
@@ -2283,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -2318,7 +2309,7 @@
         <v>59</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>14</v>
@@ -2339,10 +2330,10 @@
         <v>18</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2368,10 +2359,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>14</v>
@@ -2392,10 +2383,10 @@
         <v>18</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -2415,19 +2406,19 @@
     </row>
     <row r="25" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="4">
         <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>15</v>
@@ -2442,15 +2433,17 @@
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M25" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -2468,16 +2461,16 @@
     </row>
     <row r="26" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="4">
         <v>17</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>25</v>
@@ -2495,17 +2488,15 @@
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>65</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -2532,10 +2523,10 @@
         <v>67</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>15</v>
@@ -2553,10 +2544,10 @@
         <v>18</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -2585,7 +2576,7 @@
         <v>69</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
@@ -2606,12 +2597,14 @@
         <v>18</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="M28" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2629,16 +2622,16 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="4">
         <v>17</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
@@ -2656,17 +2649,15 @@
         <v>1</v>
       </c>
       <c r="J29" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -2693,7 +2684,7 @@
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>14</v>
@@ -2714,10 +2705,10 @@
         <v>0</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2746,7 +2737,7 @@
         <v>76</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>14</v>
@@ -2767,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2799,7 +2790,7 @@
         <v>78</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>14</v>
@@ -2820,10 +2811,10 @@
         <v>0</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2852,7 +2843,7 @@
         <v>80</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>14</v>
@@ -2861,7 +2852,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H33" s="4">
         <v>5</v>
@@ -2873,10 +2864,10 @@
         <v>0</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2905,7 +2896,7 @@
         <v>82</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>14</v>
@@ -2926,10 +2917,10 @@
         <v>0</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2958,7 +2949,7 @@
         <v>84</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>14</v>
@@ -2967,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
@@ -2979,10 +2970,10 @@
         <v>0</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -3011,7 +3002,7 @@
         <v>86</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>14</v>
@@ -3032,10 +3023,10 @@
         <v>0</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -3064,7 +3055,7 @@
         <v>88</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>14</v>
@@ -3073,7 +3064,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
@@ -3085,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -3117,7 +3108,7 @@
         <v>90</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>14</v>
@@ -3126,7 +3117,7 @@
         <v>15</v>
       </c>
       <c r="G38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
@@ -3141,7 +3132,7 @@
         <v>16</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3170,7 +3161,7 @@
         <v>92</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>14</v>
@@ -3191,10 +3182,10 @@
         <v>0</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -3223,7 +3214,7 @@
         <v>94</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>14</v>
@@ -3244,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -3276,7 +3267,7 @@
         <v>96</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>14</v>
@@ -3300,7 +3291,7 @@
         <v>16</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -3329,7 +3320,7 @@
         <v>98</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>14</v>
@@ -3353,9 +3344,11 @@
         <v>16</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M42" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
@@ -3382,7 +3375,7 @@
         <v>100</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>14</v>
@@ -3406,11 +3399,9 @@
         <v>16</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="M43" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
@@ -3437,7 +3428,7 @@
         <v>102</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>14</v>
@@ -3461,7 +3452,7 @@
         <v>16</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -3490,7 +3481,7 @@
         <v>104</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>14</v>
@@ -3514,7 +3505,7 @@
         <v>16</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
@@ -3543,7 +3534,7 @@
         <v>106</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>14</v>
@@ -3564,10 +3555,10 @@
         <v>0</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -3586,42 +3577,18 @@
       <c r="AA46" s="4"/>
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" s="4">
-        <v>17</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="H47" s="4">
-        <v>5</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L47" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -31304,53 +31271,252 @@
       <c r="Z1001" s="4"/>
       <c r="AA1001" s="4"/>
     </row>
-    <row r="1002" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1002" s="4"/>
-      <c r="B1002" s="4"/>
-      <c r="C1002" s="5"/>
-      <c r="D1002" s="4"/>
-      <c r="E1002" s="4"/>
-      <c r="F1002" s="6"/>
-      <c r="G1002" s="4"/>
-      <c r="H1002" s="4"/>
-      <c r="I1002" s="4"/>
-      <c r="J1002" s="4"/>
-      <c r="K1002" s="6"/>
-      <c r="L1002" s="6"/>
-      <c r="M1002" s="4"/>
-      <c r="N1002" s="4"/>
-      <c r="O1002" s="4"/>
-      <c r="P1002" s="4"/>
-      <c r="Q1002" s="4"/>
-      <c r="R1002" s="4"/>
-      <c r="S1002" s="4"/>
-      <c r="T1002" s="4"/>
-      <c r="U1002" s="4"/>
-      <c r="V1002" s="4"/>
-      <c r="W1002" s="4"/>
-      <c r="X1002" s="4"/>
-      <c r="Y1002" s="4"/>
-      <c r="Z1002" s="4"/>
-      <c r="AA1002" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L1002">
+  <conditionalFormatting sqref="A2:L1001">
     <cfRule type="expression" dxfId="48" priority="2">
       <formula>$K2="adj"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:L1002">
+  <conditionalFormatting sqref="A2:L1001">
     <cfRule type="expression" dxfId="47" priority="3">
       <formula>$K2="buff"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:L1002">
+  <conditionalFormatting sqref="A2:L1001">
     <cfRule type="expression" dxfId="46" priority="4">
       <formula>$K2="main"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1002">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="F29:H32 F27:J28">
+    <cfRule type="expression" dxfId="45" priority="6">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:H32 F27:J28">
+    <cfRule type="expression" dxfId="44" priority="7">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:H32 F27:J28">
+    <cfRule type="expression" dxfId="43" priority="8">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41:H42 F33:H39">
+    <cfRule type="expression" dxfId="42" priority="10">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41:H42 F33:H39">
+    <cfRule type="expression" dxfId="41" priority="11">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41:H42 F33:H39">
+    <cfRule type="expression" dxfId="40" priority="12">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40:H40">
+    <cfRule type="expression" dxfId="39" priority="13">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40:H40">
+    <cfRule type="expression" dxfId="38" priority="14">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40:H40">
+    <cfRule type="expression" dxfId="37" priority="15">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="36" priority="16">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="35" priority="17">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="34" priority="18">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="33" priority="19">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="32" priority="20">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:H43">
+    <cfRule type="expression" dxfId="31" priority="21">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="30" priority="22">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="29" priority="23">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="28" priority="24">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:H44">
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="24" priority="28">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="23" priority="29">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="22" priority="30">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="21" priority="31">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="20" priority="32">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:H45">
+    <cfRule type="expression" dxfId="19" priority="33">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="18" priority="34">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="17" priority="35">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="16" priority="36">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="15" priority="37">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="14" priority="38">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:H46">
+    <cfRule type="expression" dxfId="13" priority="39">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="12" priority="40">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="11" priority="41">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="10" priority="42">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="9" priority="43">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="8" priority="44">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:H47">
+    <cfRule type="expression" dxfId="7" priority="45">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="6" priority="46">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="5" priority="47">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="4" priority="48">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="3" priority="49">
+      <formula>#REF!="adj"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="2" priority="50">
+      <formula>#REF!="buff"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:H48">
+    <cfRule type="expression" dxfId="1" priority="51">
+      <formula>#REF!="main"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1001">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31361,23 +31527,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="45" priority="6">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="44" priority="7">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:H33 F28:J29">
-    <cfRule type="expression" dxfId="43" priority="8">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1002">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="B1:B1001">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31388,219 +31539,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="42" priority="10">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="41" priority="11">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42:H43 F34:H40">
-    <cfRule type="expression" dxfId="40" priority="12">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="39" priority="13">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="38" priority="14">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41:H41">
-    <cfRule type="expression" dxfId="37" priority="15">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="36" priority="16">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="35" priority="17">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="34" priority="18">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="33" priority="19">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="32" priority="20">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:H44">
-    <cfRule type="expression" dxfId="31" priority="21">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="30" priority="22">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="29" priority="23">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="28" priority="24">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="27" priority="25">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="26" priority="26">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:H45">
-    <cfRule type="expression" dxfId="25" priority="27">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="24" priority="28">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="23" priority="29">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="22" priority="30">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="21" priority="31">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="20" priority="32">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:H46">
-    <cfRule type="expression" dxfId="19" priority="33">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="18" priority="34">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="17" priority="35">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="16" priority="36">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="15" priority="37">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="14" priority="38">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:H47">
-    <cfRule type="expression" dxfId="13" priority="39">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="12" priority="40">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="11" priority="41">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="10" priority="42">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="9" priority="43">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="8" priority="44">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48:H48">
-    <cfRule type="expression" dxfId="7" priority="45">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="6" priority="46">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="5" priority="47">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="4" priority="48">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="3" priority="49">
-      <formula>#REF!="adj"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="2" priority="50">
-      <formula>#REF!="buff"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:H49">
-    <cfRule type="expression" dxfId="1" priority="51">
-      <formula>#REF!="main"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
updated dates to fix agrucaras adj
</commit_message>
<xml_diff>
--- a/dataset/17_ROIs.xlsx
+++ b/dataset/17_ROIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3E8A3-4B2D-438C-BDE5-2B21F3C5D55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B87BC4-6508-4E30-AC27-70F33F48B38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROIs" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1241,7 +1241,7 @@
         <v>118</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1250,7 +1250,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4">
         <v>5</v>
@@ -1400,7 +1400,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>14</v>
@@ -1409,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
         <v>5</v>

</xml_diff>